<commit_message>
Updated packages and code
</commit_message>
<xml_diff>
--- a/BIM_Automation/src/main/java/bil/resources/Automation-TestData.xlsx
+++ b/BIM_Automation/src/main/java/bil/resources/Automation-TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/private/var/mobile/Containers/Data/Application/363AF7B7-7DCC-4ECC-9301-12EE237A51B8/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/private/var/mobile/Containers/Data/Application/BEE77911-87BD-4ABE-8568-B66062A9D04B/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60A81CA4-C84C-6B4C-B42A-0CF0E5382400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21B8D47D-A636-1D45-BD2D-51A6DE5C34C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MRLTeacherLogin" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="StudentRegistration" sheetId="10" r:id="rId10"/>
     <sheet name="DARegistration" sheetId="11" r:id="rId11"/>
     <sheet name="MultipleStudentRegistration" sheetId="12" r:id="rId12"/>
-    <sheet name="MultipleTeacherRegistration" sheetId="13" r:id="rId13"/>
+    <sheet name="MultipleTeacherRegistration" sheetId="19" r:id="rId13"/>
     <sheet name="MultipleDARegistration" sheetId="14" r:id="rId14"/>
     <sheet name="AddClassForNewUser" sheetId="15" r:id="rId15"/>
     <sheet name="AddClassWhenNoActiveClass" sheetId="16" r:id="rId16"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="61">
   <si>
     <t>USERNAME</t>
   </si>
@@ -212,6 +212,9 @@
     <t>BOOK</t>
   </si>
   <si>
+    <t>mutlipleauto0.teacher00883@zeus.com</t>
+  </si>
+  <si>
     <t>FirstGradeClass</t>
   </si>
   <si>
@@ -221,13 +224,13 @@
     <t>Grade 1: MRL</t>
   </si>
   <si>
+    <t>mutliauto1.teacher15206@zeus.com</t>
+  </si>
+  <si>
     <t>autotest2.teacher@zeus.com</t>
   </si>
   <si>
-    <t>Pbztest1@zeus.com</t>
-  </si>
-  <si>
-    <t>Pbztest2@zeus.com</t>
+    <t>2EAE-PTBR-KJHH</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,19 +299,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -316,9 +310,7 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -342,14 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -358,11 +343,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -383,27 +367,16 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -4837,7 +4810,7 @@
     <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4847,18 +4820,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:E998"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72B4DE9-AA9A-5640-BEEC-AD0878634E16}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="27.58203125" customWidth="1"/>
-    <col min="2" max="25" width="8.578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -4875,9 +4846,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>44</v>
@@ -4888,1020 +4859,12 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>46</v>
+      <c r="E2" s="5">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(E2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6965,9 +5928,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6975,55 +5936,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>59</v>
+      <c r="A2" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="19">
-        <v>43485</v>
-      </c>
-      <c r="F2" s="19">
-        <v>45432</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="D2" s="5" t="s">
         <v>56</v>
+      </c>
+      <c r="E2" s="18">
+        <v>44256</v>
+      </c>
+      <c r="F2" s="18">
+        <v>44377</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6211581A-4E99-6F47-90A2-0D8D9234FB58}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7035,62 +5993,57 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="21">
+        <v>56</v>
+      </c>
+      <c r="E2" s="18">
         <v>44256</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="18">
         <v>44377</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{021B0582-FF9C-E74B-8E35-7FA0BD852223}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7102,9 +6055,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7112,55 +6063,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>57</v>
+      <c r="A2" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="21">
+        <v>56</v>
+      </c>
+      <c r="E2" s="18">
         <v>44256</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="18">
         <v>44377</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{450654E6-D053-EC4D-8C52-2E29BC084B2A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>